<commit_message>
feat: #108 Re-generate the statistics with the fixed minutes and seconds formatting in the haul fields. It affects both html and excel files.
</commit_message>
<xml_diff>
--- a/kgstats-generated/2024.11.11/stats/xlsx/voc-14878-top-by-best-speed.xlsx
+++ b/kgstats-generated/2024.11.11/stats/xlsx/voc-14878-top-by-best-speed.xlsx
@@ -77,7 +77,7 @@
     <t>fivestar</t>
   </si>
   <si>
-    <t>9 ч. 5 мин. 21 сек.</t>
+    <t>9 ч. 05 мин. 21 сек.</t>
   </si>
   <si>
     <t>5</t>
@@ -104,7 +104,7 @@
     <t>Vielle</t>
   </si>
   <si>
-    <t>0 ч. 31 мин. 0 сек.</t>
+    <t>0 ч. 31 мин. 00 сек.</t>
   </si>
   <si>
     <t>8</t>
@@ -131,7 +131,7 @@
     <t>Виталька</t>
   </si>
   <si>
-    <t>2 ч. 17 мин. 5 сек.</t>
+    <t>2 ч. 17 мин. 05 сек.</t>
   </si>
   <si>
     <t>11–12</t>
@@ -140,13 +140,13 @@
     <t>vei</t>
   </si>
   <si>
-    <t>1 ч. 1 мин. 11 сек.</t>
+    <t>1 ч. 01 мин. 11 сек.</t>
   </si>
   <si>
     <t>Speedyman</t>
   </si>
   <si>
-    <t>5 ч. 29 мин. 7 сек.</t>
+    <t>5 ч. 29 мин. 07 сек.</t>
   </si>
   <si>
     <t>13</t>
@@ -182,7 +182,7 @@
     <t>170000</t>
   </si>
   <si>
-    <t>9 ч. 6 мин. 27 сек.</t>
+    <t>9 ч. 06 мин. 27 сек.</t>
   </si>
   <si>
     <t>17</t>
@@ -200,7 +200,7 @@
     <t>s0lnyshk0</t>
   </si>
   <si>
-    <t>2 ч. 3 мин. 54 сек.</t>
+    <t>2 ч. 03 мин. 54 сек.</t>
   </si>
   <si>
     <t>19</t>
@@ -218,7 +218,7 @@
     <t>Mellow</t>
   </si>
   <si>
-    <t>1 ч. 4 мин. 32 сек.</t>
+    <t>1 ч. 04 мин. 32 сек.</t>
   </si>
   <si>
     <t>21</t>
@@ -254,7 +254,7 @@
     <t>chikaldirick</t>
   </si>
   <si>
-    <t>0 ч. 20 мин. 4 сек.</t>
+    <t>0 ч. 20 мин. 04 сек.</t>
   </si>
   <si>
     <t>25</t>
@@ -296,7 +296,7 @@
     <t>fatuous</t>
   </si>
   <si>
-    <t>1 ч. 53 мин. 3 сек.</t>
+    <t>1 ч. 53 мин. 03 сек.</t>
   </si>
   <si>
     <t>30</t>
@@ -332,7 +332,7 @@
     <t>spawn_once</t>
   </si>
   <si>
-    <t>1 ч. 27 мин. 0 сек.</t>
+    <t>1 ч. 27 мин. 00 сек.</t>
   </si>
   <si>
     <t>34</t>
@@ -359,7 +359,7 @@
     <t>M87</t>
   </si>
   <si>
-    <t>2 ч. 7 мин. 5 сек.</t>
+    <t>2 ч. 07 мин. 05 сек.</t>
   </si>
   <si>
     <t>37</t>
@@ -377,7 +377,7 @@
     <t>shdw</t>
   </si>
   <si>
-    <t>0 ч. 39 мин. 4 сек.</t>
+    <t>0 ч. 39 мин. 04 сек.</t>
   </si>
   <si>
     <t>Evariste</t>
@@ -392,7 +392,7 @@
     <t>Arimusya</t>
   </si>
   <si>
-    <t>1 ч. 1 мин. 54 сек.</t>
+    <t>1 ч. 01 мин. 54 сек.</t>
   </si>
   <si>
     <t>еаеа</t>
@@ -407,7 +407,7 @@
     <t>sashavirtual</t>
   </si>
   <si>
-    <t>1 ч. 31 мин. 3 сек.</t>
+    <t>1 ч. 31 мин. 03 сек.</t>
   </si>
   <si>
     <t>43</t>
@@ -479,7 +479,7 @@
     <t>oyasumi</t>
   </si>
   <si>
-    <t>1 ч. 51 мин. 8 сек.</t>
+    <t>1 ч. 51 мин. 08 сек.</t>
   </si>
   <si>
     <t>51</t>
@@ -530,7 +530,7 @@
     <t>Толик_Цой</t>
   </si>
   <si>
-    <t>1 ч. 14 мин. 1 сек.</t>
+    <t>1 ч. 14 мин. 01 сек.</t>
   </si>
   <si>
     <t>57</t>
@@ -593,7 +593,7 @@
     <t>кляпавций</t>
   </si>
   <si>
-    <t>0 ч. 28 мин. 3 сек.</t>
+    <t>0 ч. 28 мин. 03 сек.</t>
   </si>
   <si>
     <t>64–65</t>
@@ -626,7 +626,7 @@
     <t>mdnf</t>
   </si>
   <si>
-    <t>3 ч. 3 мин. 34 сек.</t>
+    <t>3 ч. 03 мин. 34 сек.</t>
   </si>
   <si>
     <t>68</t>
@@ -650,7 +650,7 @@
     <t>MaestroPain</t>
   </si>
   <si>
-    <t>28 ч. 4 мин. 11 сек.</t>
+    <t>28 ч. 04 мин. 11 сек.</t>
   </si>
   <si>
     <t>71–72</t>
@@ -659,13 +659,13 @@
     <t>AstonMartinDB10</t>
   </si>
   <si>
-    <t>2 ч. 15 мин. 8 сек.</t>
+    <t>2 ч. 15 мин. 08 сек.</t>
   </si>
   <si>
     <t>Just</t>
   </si>
   <si>
-    <t>1 ч. 9 мин. 1 сек.</t>
+    <t>1 ч. 09 мин. 01 сек.</t>
   </si>
   <si>
     <t>73–74</t>
@@ -722,7 +722,7 @@
     <t>Denzilman</t>
   </si>
   <si>
-    <t>1 ч. 6 мин. 13 сек.</t>
+    <t>1 ч. 06 мин. 13 сек.</t>
   </si>
   <si>
     <t>80</t>
@@ -758,7 +758,7 @@
     <t>molot-perm</t>
   </si>
   <si>
-    <t>6 ч. 6 мин. 52 сек.</t>
+    <t>6 ч. 06 мин. 52 сек.</t>
   </si>
   <si>
     <t>84</t>
@@ -785,7 +785,7 @@
     <t>паукан</t>
   </si>
   <si>
-    <t>86 ч. 16 мин. 9 сек.</t>
+    <t>86 ч. 16 мин. 09 сек.</t>
   </si>
   <si>
     <t>87</t>
@@ -794,7 +794,7 @@
     <t>Etoneja</t>
   </si>
   <si>
-    <t>1 ч. 0 мин. 42 сек.</t>
+    <t>1 ч. 00 мин. 42 сек.</t>
   </si>
   <si>
     <t>88</t>
@@ -803,7 +803,7 @@
     <t>_Nicole_</t>
   </si>
   <si>
-    <t>2 ч. 5 мин. 58 сек.</t>
+    <t>2 ч. 05 мин. 58 сек.</t>
   </si>
   <si>
     <t>89–90</t>
@@ -812,7 +812,7 @@
     <t>4bia</t>
   </si>
   <si>
-    <t>0 ч. 53 мин. 6 сек.</t>
+    <t>0 ч. 53 мин. 06 сек.</t>
   </si>
   <si>
     <t>Сельтик</t>
@@ -827,7 +827,7 @@
     <t>strix_qb</t>
   </si>
   <si>
-    <t>2 ч. 11 мин. 8 сек.</t>
+    <t>2 ч. 11 мин. 08 сек.</t>
   </si>
   <si>
     <t>пипеткин</t>
@@ -860,7 +860,7 @@
     <t>system_error</t>
   </si>
   <si>
-    <t>1 ч. 25 мин. 6 сек.</t>
+    <t>1 ч. 25 мин. 06 сек.</t>
   </si>
   <si>
     <t>96</t>
@@ -896,7 +896,7 @@
     <t>Ludimagister</t>
   </si>
   <si>
-    <t>1 ч. 2 мин. 56 сек.</t>
+    <t>1 ч. 02 мин. 56 сек.</t>
   </si>
   <si>
     <t>TypeError</t>
@@ -926,7 +926,7 @@
     <t>AlexUnder</t>
   </si>
   <si>
-    <t>0 ч. 31 мин. 4 сек.</t>
+    <t>0 ч. 31 мин. 04 сек.</t>
   </si>
   <si>
     <t>Cybernetix</t>
@@ -947,13 +947,13 @@
     <t>mynque</t>
   </si>
   <si>
-    <t>0 ч. 25 мин. 9 сек.</t>
+    <t>0 ч. 25 мин. 09 сек.</t>
   </si>
   <si>
     <t>Fenex</t>
   </si>
   <si>
-    <t>1 ч. 5 мин. 52 сек.</t>
+    <t>1 ч. 05 мин. 52 сек.</t>
   </si>
   <si>
     <t>zhtw</t>
@@ -968,13 +968,13 @@
     <t>Static</t>
   </si>
   <si>
-    <t>2 ч. 7 мин. 4 сек.</t>
+    <t>2 ч. 07 мин. 04 сек.</t>
   </si>
   <si>
     <t>Phemmer</t>
   </si>
   <si>
-    <t>11 ч. 7 мин. 9 сек.</t>
+    <t>11 ч. 07 мин. 09 сек.</t>
   </si>
   <si>
     <t>111</t>
@@ -983,7 +983,7 @@
     <t>КлавоЕд</t>
   </si>
   <si>
-    <t>1 ч. 5 мин. 28 сек.</t>
+    <t>1 ч. 05 мин. 28 сек.</t>
   </si>
   <si>
     <t>112</t>
@@ -1010,7 +1010,7 @@
     <t>Экстравагантный</t>
   </si>
   <si>
-    <t>1 ч. 21 мин. 8 сек.</t>
+    <t>1 ч. 21 мин. 08 сек.</t>
   </si>
   <si>
     <t>Dimanus</t>
@@ -1031,7 +1031,7 @@
     <t>Gal04ka</t>
   </si>
   <si>
-    <t>11 ч. 2 мин. 6 сек.</t>
+    <t>11 ч. 02 мин. 06 сек.</t>
   </si>
   <si>
     <t>118–119</t>
@@ -1046,7 +1046,7 @@
     <t>Enrage</t>
   </si>
   <si>
-    <t>5 ч. 10 мин. 9 сек.</t>
+    <t>5 ч. 10 мин. 09 сек.</t>
   </si>
   <si>
     <t>120–121</t>
@@ -1055,7 +1055,7 @@
     <t>bulatenkom</t>
   </si>
   <si>
-    <t>3 ч. 23 мин. 1 сек.</t>
+    <t>3 ч. 23 мин. 01 сек.</t>
   </si>
   <si>
     <t>Mediator</t>
@@ -1133,7 +1133,7 @@
     <t>FarWin</t>
   </si>
   <si>
-    <t>25 ч. 23 мин. 9 сек.</t>
+    <t>25 ч. 23 мин. 09 сек.</t>
   </si>
   <si>
     <t>131–134</t>
@@ -1142,7 +1142,7 @@
     <t>exdark</t>
   </si>
   <si>
-    <t>1 ч. 2 мин. 10 сек.</t>
+    <t>1 ч. 02 мин. 10 сек.</t>
   </si>
   <si>
     <t>libertadore</t>
@@ -1154,13 +1154,13 @@
     <t>saben_askhat</t>
   </si>
   <si>
-    <t>3 ч. 5 мин. 12 сек.</t>
+    <t>3 ч. 05 мин. 12 сек.</t>
   </si>
   <si>
     <t>haos2100</t>
   </si>
   <si>
-    <t>4 ч. 7 мин. 51 сек.</t>
+    <t>4 ч. 07 мин. 51 сек.</t>
   </si>
   <si>
     <t>135–137</t>
@@ -1169,19 +1169,19 @@
     <t>бэтман</t>
   </si>
   <si>
-    <t>2 ч. 6 мин. 47 сек.</t>
+    <t>2 ч. 06 мин. 47 сек.</t>
   </si>
   <si>
     <t>mavru</t>
   </si>
   <si>
-    <t>2 ч. 2 мин. 57 сек.</t>
+    <t>2 ч. 02 мин. 57 сек.</t>
   </si>
   <si>
     <t>valeryani</t>
   </si>
   <si>
-    <t>4 ч. 35 мин. 8 сек.</t>
+    <t>4 ч. 35 мин. 08 сек.</t>
   </si>
   <si>
     <t>138–139</t>
@@ -1238,13 +1238,13 @@
     <t>Desser</t>
   </si>
   <si>
-    <t>1 ч. 9 мин. 54 сек.</t>
+    <t>1 ч. 09 мин. 54 сек.</t>
   </si>
   <si>
     <t>deadmage</t>
   </si>
   <si>
-    <t>1 ч. 34 мин. 6 сек.</t>
+    <t>1 ч. 34 мин. 06 сек.</t>
   </si>
   <si>
     <t>146</t>
@@ -1277,7 +1277,7 @@
     <t>Oyvse</t>
   </si>
   <si>
-    <t>1 ч. 2 мин. 40 сек.</t>
+    <t>1 ч. 02 мин. 40 сек.</t>
   </si>
   <si>
     <t>150–152</t>
@@ -1292,7 +1292,7 @@
     <t>igormsu</t>
   </si>
   <si>
-    <t>1 ч. 52 мин. 0 сек.</t>
+    <t>1 ч. 52 мин. 00 сек.</t>
   </si>
   <si>
     <t>Lil-Cut-Throat</t>
@@ -1355,7 +1355,7 @@
     <t>LANC</t>
   </si>
   <si>
-    <t>1 ч. 0 мин. 49 сек.</t>
+    <t>1 ч. 00 мин. 49 сек.</t>
   </si>
   <si>
     <t>160–162</t>
@@ -1370,7 +1370,7 @@
     <t>ИльдарВолжский</t>
   </si>
   <si>
-    <t>1 ч. 5 мин. 56 сек.</t>
+    <t>1 ч. 05 мин. 56 сек.</t>
   </si>
   <si>
     <t>Arsen27</t>
@@ -1385,13 +1385,13 @@
     <t>batkovich</t>
   </si>
   <si>
-    <t>0 ч. 45 мин. 8 сек.</t>
+    <t>0 ч. 45 мин. 08 сек.</t>
   </si>
   <si>
     <t>NDancer</t>
   </si>
   <si>
-    <t>0 ч. 40 мин. 6 сек.</t>
+    <t>0 ч. 40 мин. 06 сек.</t>
   </si>
   <si>
     <t>165–166</t>
@@ -1451,13 +1451,13 @@
     <t>Bolot</t>
   </si>
   <si>
-    <t>1 ч. 25 мин. 7 сек.</t>
+    <t>1 ч. 25 мин. 07 сек.</t>
   </si>
   <si>
     <t>lovermann</t>
   </si>
   <si>
-    <t>2 ч. 3 мин. 26 сек.</t>
+    <t>2 ч. 03 мин. 26 сек.</t>
   </si>
   <si>
     <t>174–175</t>
@@ -1472,7 +1472,7 @@
     <t>Bhiopk</t>
   </si>
   <si>
-    <t>1 ч. 5 мин. 21 сек.</t>
+    <t>1 ч. 05 мин. 21 сек.</t>
   </si>
   <si>
     <t>176–177</t>
@@ -1496,7 +1496,7 @@
     <t>droom</t>
   </si>
   <si>
-    <t>1 ч. 7 мин. 33 сек.</t>
+    <t>1 ч. 07 мин. 33 сек.</t>
   </si>
   <si>
     <t>179</t>
@@ -1505,7 +1505,7 @@
     <t>PROcent</t>
   </si>
   <si>
-    <t>2 ч. 5 мин. 40 сек.</t>
+    <t>2 ч. 05 мин. 40 сек.</t>
   </si>
   <si>
     <t>180</t>
@@ -1538,7 +1538,7 @@
     <t>Ferris</t>
   </si>
   <si>
-    <t>0 ч. 36 мин. 5 сек.</t>
+    <t>0 ч. 36 мин. 05 сек.</t>
   </si>
   <si>
     <t>Loyaluna</t>
@@ -1580,7 +1580,7 @@
     <t>puchkarito</t>
   </si>
   <si>
-    <t>1 ч. 46 мин. 6 сек.</t>
+    <t>1 ч. 46 мин. 06 сек.</t>
   </si>
   <si>
     <t>190</t>
@@ -1634,7 +1634,7 @@
     <t>Обгоняша</t>
   </si>
   <si>
-    <t>8 ч. 24 мин. 4 сек.</t>
+    <t>8 ч. 24 мин. 04 сек.</t>
   </si>
   <si>
     <t>197</t>
@@ -1658,7 +1658,7 @@
     <t>VisaryMaster</t>
   </si>
   <si>
-    <t>3 ч. 0 мин. 33 сек.</t>
+    <t>3 ч. 00 мин. 33 сек.</t>
   </si>
   <si>
     <t>Cherrik</t>
@@ -1691,7 +1691,7 @@
     <t>Satory</t>
   </si>
   <si>
-    <t>11 ч. 6 мин. 25 сек.</t>
+    <t>11 ч. 06 мин. 25 сек.</t>
   </si>
   <si>
     <t>205–207</t>
@@ -1712,7 +1712,7 @@
     <t>serega__</t>
   </si>
   <si>
-    <t>0 ч. 47 мин. 1 сек.</t>
+    <t>0 ч. 47 мин. 01 сек.</t>
   </si>
   <si>
     <t>208</t>
@@ -1745,13 +1745,13 @@
     <t>sav1</t>
   </si>
   <si>
-    <t>1 ч. 27 мин. 8 сек.</t>
+    <t>1 ч. 27 мин. 08 сек.</t>
   </si>
   <si>
     <t>vIRwO</t>
   </si>
   <si>
-    <t>6 ч. 29 мин. 1 сек.</t>
+    <t>6 ч. 29 мин. 01 сек.</t>
   </si>
   <si>
     <t>213–214</t>
@@ -1802,7 +1802,7 @@
     <t>MrSir</t>
   </si>
   <si>
-    <t>4 ч. 47 мин. 5 сек.</t>
+    <t>4 ч. 47 мин. 05 сек.</t>
   </si>
   <si>
     <t>HeLLios</t>
@@ -1883,7 +1883,7 @@
     <t>Хаотический</t>
   </si>
   <si>
-    <t>12 ч. 8 мин. 34 сек.</t>
+    <t>12 ч. 08 мин. 34 сек.</t>
   </si>
   <si>
     <t>erfectionist</t>
@@ -1949,13 +1949,13 @@
     <t>CroW1985</t>
   </si>
   <si>
-    <t>0 ч. 40 мин. 1 сек.</t>
+    <t>0 ч. 40 мин. 01 сек.</t>
   </si>
   <si>
     <t>qwertrewq</t>
   </si>
   <si>
-    <t>1 ч. 35 мин. 9 сек.</t>
+    <t>1 ч. 35 мин. 09 сек.</t>
   </si>
   <si>
     <t>241</t>
@@ -1997,7 +1997,7 @@
     <t>Disobey</t>
   </si>
   <si>
-    <t>1 ч. 28 мин. 8 сек.</t>
+    <t>1 ч. 28 мин. 08 сек.</t>
   </si>
   <si>
     <t>246–247</t>
@@ -2012,7 +2012,7 @@
     <t>pche1</t>
   </si>
   <si>
-    <t>5 ч. 2 мин. 43 сек.</t>
+    <t>5 ч. 02 мин. 43 сек.</t>
   </si>
   <si>
     <t>248–256</t>
@@ -2027,13 +2027,13 @@
     <t>sneg_jr</t>
   </si>
   <si>
-    <t>0 ч. 38 мин. 3 сек.</t>
+    <t>0 ч. 38 мин. 03 сек.</t>
   </si>
   <si>
     <t>Gr1nch</t>
   </si>
   <si>
-    <t>0 ч. 38 мин. 7 сек.</t>
+    <t>0 ч. 38 мин. 07 сек.</t>
   </si>
   <si>
     <t>Джиперс_Криперс</t>
@@ -2045,7 +2045,7 @@
     <t>Euki</t>
   </si>
   <si>
-    <t>1 ч. 7 мин. 11 сек.</t>
+    <t>1 ч. 07 мин. 11 сек.</t>
   </si>
   <si>
     <t>petrovich</t>
@@ -2069,7 +2069,7 @@
     <t>Glavredzlovred</t>
   </si>
   <si>
-    <t>6 ч. 43 мин. 0 сек.</t>
+    <t>6 ч. 43 мин. 00 сек.</t>
   </si>
   <si>
     <t>257–258</t>
@@ -2123,7 +2123,7 @@
     <t>MarionWed</t>
   </si>
   <si>
-    <t>20 ч. 6 мин. 55 сек.</t>
+    <t>20 ч. 06 мин. 55 сек.</t>
   </si>
   <si>
     <t>264–265</t>
@@ -2231,7 +2231,7 @@
     <t>stag_</t>
   </si>
   <si>
-    <t>5 ч. 5 мин. 19 сек.</t>
+    <t>5 ч. 05 мин. 19 сек.</t>
   </si>
   <si>
     <t>280</t>
@@ -2249,7 +2249,7 @@
     <t>Breakdown</t>
   </si>
   <si>
-    <t>1 ч. 2 мин. 23 сек.</t>
+    <t>1 ч. 02 мин. 23 сек.</t>
   </si>
   <si>
     <t>jacknov</t>
@@ -2288,7 +2288,7 @@
     <t>Себрик</t>
   </si>
   <si>
-    <t>1 ч. 8 мин. 4 сек.</t>
+    <t>1 ч. 08 мин. 04 сек.</t>
   </si>
   <si>
     <t>drummer_type</t>
@@ -2300,7 +2300,7 @@
     <t>NightKlirik</t>
   </si>
   <si>
-    <t>2 ч. 35 мин. 8 сек.</t>
+    <t>2 ч. 35 мин. 08 сек.</t>
   </si>
   <si>
     <t>290–293</t>
@@ -2315,13 +2315,13 @@
     <t>SpazZm</t>
   </si>
   <si>
-    <t>0 ч. 35 мин. 6 сек.</t>
+    <t>0 ч. 35 мин. 06 сек.</t>
   </si>
   <si>
     <t>MMikhotov</t>
   </si>
   <si>
-    <t>0 ч. 41 мин. 6 сек.</t>
+    <t>0 ч. 41 мин. 06 сек.</t>
   </si>
   <si>
     <t>Syper_fast</t>
@@ -2336,19 +2336,19 @@
     <t>galileo-job</t>
   </si>
   <si>
-    <t>1 ч. 0 мин. 38 сек.</t>
+    <t>1 ч. 00 мин. 38 сек.</t>
   </si>
   <si>
     <t>Locust</t>
   </si>
   <si>
-    <t>1 ч. 4 мин. 57 сек.</t>
+    <t>1 ч. 04 мин. 57 сек.</t>
   </si>
   <si>
     <t>iChessKnock</t>
   </si>
   <si>
-    <t>3 ч. 14 мин. 3 сек.</t>
+    <t>3 ч. 14 мин. 03 сек.</t>
   </si>
   <si>
     <t>Insane_Grinder</t>
@@ -2369,7 +2369,7 @@
     <t>lxndrdnlv</t>
   </si>
   <si>
-    <t>1 ч. 40 мин. 0 сек.</t>
+    <t>1 ч. 40 мин. 00 сек.</t>
   </si>
   <si>
     <t>SpiritCrusher</t>
@@ -2405,7 +2405,7 @@
     <t>MrFlag</t>
   </si>
   <si>
-    <t>0 ч. 42 мин. 0 сек.</t>
+    <t>0 ч. 42 мин. 00 сек.</t>
   </si>
   <si>
     <t>305–307</t>
@@ -2480,13 +2480,13 @@
     <t>NionNet</t>
   </si>
   <si>
-    <t>1 ч. 6 мин. 15 сек.</t>
+    <t>1 ч. 06 мин. 15 сек.</t>
   </si>
   <si>
     <t>Nowhereman42nd</t>
   </si>
   <si>
-    <t>4 ч. 11 мин. 6 сек.</t>
+    <t>4 ч. 11 мин. 06 сек.</t>
   </si>
   <si>
     <t>Sonick071</t>
@@ -2501,7 +2501,7 @@
     <t>Wantnonick</t>
   </si>
   <si>
-    <t>0 ч. 50 мин. 9 сек.</t>
+    <t>0 ч. 50 мин. 09 сек.</t>
   </si>
   <si>
     <t>hyperX</t>
@@ -2546,25 +2546,25 @@
     <t>dbz</t>
   </si>
   <si>
-    <t>2 ч. 7 мин. 23 сек.</t>
+    <t>2 ч. 07 мин. 23 сек.</t>
   </si>
   <si>
     <t>dsdt</t>
   </si>
   <si>
-    <t>2 ч. 3 мин. 24 сек.</t>
+    <t>2 ч. 03 мин. 24 сек.</t>
   </si>
   <si>
     <t>я_араб</t>
   </si>
   <si>
-    <t>3 ч. 9 мин. 11 сек.</t>
+    <t>3 ч. 09 мин. 11 сек.</t>
   </si>
   <si>
     <t>Awyra</t>
   </si>
   <si>
-    <t>19 ч. 52 мин. 6 сек.</t>
+    <t>19 ч. 52 мин. 06 сек.</t>
   </si>
   <si>
     <t>328–331</t>
@@ -2615,7 +2615,7 @@
     <t>anania2003</t>
   </si>
   <si>
-    <t>0 ч. 34 мин. 0 сек.</t>
+    <t>0 ч. 34 мин. 00 сек.</t>
   </si>
   <si>
     <t>foxxy</t>
@@ -2627,7 +2627,7 @@
     <t>Uraniadz</t>
   </si>
   <si>
-    <t>2 ч. 5 мин. 22 сек.</t>
+    <t>2 ч. 05 мин. 22 сек.</t>
   </si>
   <si>
     <t>337–339</t>
@@ -2648,7 +2648,7 @@
     <t>Vsesvet</t>
   </si>
   <si>
-    <t>1 ч. 7 мин. 40 сек.</t>
+    <t>1 ч. 07 мин. 40 сек.</t>
   </si>
   <si>
     <t>340–343</t>
@@ -2669,13 +2669,13 @@
     <t>Alli-Shi</t>
   </si>
   <si>
-    <t>1 ч. 6 мин. 36 сек.</t>
+    <t>1 ч. 06 мин. 36 сек.</t>
   </si>
   <si>
     <t>Кадий</t>
   </si>
   <si>
-    <t>2 ч. 6 мин. 38 сек.</t>
+    <t>2 ч. 06 мин. 38 сек.</t>
   </si>
   <si>
     <t>344</t>
@@ -2693,7 +2693,7 @@
     <t>Аромат</t>
   </si>
   <si>
-    <t>0 ч. 52 мин. 6 сек.</t>
+    <t>0 ч. 52 мин. 06 сек.</t>
   </si>
   <si>
     <t>Руфер</t>
@@ -2708,7 +2708,7 @@
     <t>http</t>
   </si>
   <si>
-    <t>1 ч. 6 мин. 4 сек.</t>
+    <t>1 ч. 06 мин. 04 сек.</t>
   </si>
   <si>
     <t>348–349</t>
@@ -2756,7 +2756,7 @@
     <t>flethentel</t>
   </si>
   <si>
-    <t>5 ч. 8 мин. 38 сек.</t>
+    <t>5 ч. 08 мин. 38 сек.</t>
   </si>
   <si>
     <t>354–358</t>
@@ -2774,19 +2774,19 @@
     <t>dosaaf76</t>
   </si>
   <si>
-    <t>1 ч. 6 мин. 31 сек.</t>
+    <t>1 ч. 06 мин. 31 сек.</t>
   </si>
   <si>
     <t>ITur</t>
   </si>
   <si>
-    <t>2 ч. 3 мин. 15 сек.</t>
+    <t>2 ч. 03 мин. 15 сек.</t>
   </si>
   <si>
     <t>Андруша</t>
   </si>
   <si>
-    <t>8 ч. 43 мин. 4 сек.</t>
+    <t>8 ч. 43 мин. 04 сек.</t>
   </si>
   <si>
     <t>359–363</t>
@@ -2795,7 +2795,7 @@
     <t>Mish0k</t>
   </si>
   <si>
-    <t>0 ч. 32 мин. 7 сек.</t>
+    <t>0 ч. 32 мин. 07 сек.</t>
   </si>
   <si>
     <t>MorfNotFound</t>
@@ -2891,13 +2891,13 @@
     <t>RODIS</t>
   </si>
   <si>
-    <t>1 ч. 14 мин. 5 сек.</t>
+    <t>1 ч. 14 мин. 05 сек.</t>
   </si>
   <si>
     <t>Hold_Tight</t>
   </si>
   <si>
-    <t>2 ч. 33 мин. 6 сек.</t>
+    <t>2 ч. 33 мин. 06 сек.</t>
   </si>
   <si>
     <t>375</t>
@@ -2906,7 +2906,7 @@
     <t>andech</t>
   </si>
   <si>
-    <t>1 ч. 38 мин. 9 сек.</t>
+    <t>1 ч. 38 мин. 09 сек.</t>
   </si>
   <si>
     <t>376–378</t>
@@ -2921,7 +2921,7 @@
     <t>Vovaldo</t>
   </si>
   <si>
-    <t>2 ч. 8 мин. 14 сек.</t>
+    <t>2 ч. 08 мин. 14 сек.</t>
   </si>
   <si>
     <t>Lelick</t>
@@ -2960,7 +2960,7 @@
     <t>keyBoardMan</t>
   </si>
   <si>
-    <t>1 ч. 3 мин. 26 сек.</t>
+    <t>1 ч. 03 мин. 26 сек.</t>
   </si>
   <si>
     <t>Serhio97</t>
@@ -2993,7 +2993,7 @@
     <t>WellMaxT</t>
   </si>
   <si>
-    <t>1 ч. 23 мин. 4 сек.</t>
+    <t>1 ч. 23 мин. 04 сек.</t>
   </si>
   <si>
     <t>sqwerty</t>
@@ -3029,7 +3029,7 @@
     <t>Joumii</t>
   </si>
   <si>
-    <t>7 ч. 9 мин. 47 сек.</t>
+    <t>7 ч. 09 мин. 47 сек.</t>
   </si>
   <si>
     <t>Ямастер</t>
@@ -3044,7 +3044,7 @@
     <t>pik7gbv</t>
   </si>
   <si>
-    <t>6 ч. 43 мин. 2 сек.</t>
+    <t>6 ч. 43 мин. 02 сек.</t>
   </si>
   <si>
     <t>xlsx</t>
@@ -3059,7 +3059,7 @@
     <t>Adygha</t>
   </si>
   <si>
-    <t>0 ч. 44 мин. 6 сек.</t>
+    <t>0 ч. 44 мин. 06 сек.</t>
   </si>
   <si>
     <t>элля</t>
@@ -3080,7 +3080,7 @@
     <t>Noel</t>
   </si>
   <si>
-    <t>2 ч. 8 мин. 11 сек.</t>
+    <t>2 ч. 08 мин. 11 сек.</t>
   </si>
   <si>
     <t>401–403</t>
@@ -3098,7 +3098,7 @@
     <t>Iterator</t>
   </si>
   <si>
-    <t>5 ч. 7 мин. 43 сек.</t>
+    <t>5 ч. 07 мин. 43 сек.</t>
   </si>
   <si>
     <t>404–408</t>
@@ -3107,7 +3107,7 @@
     <t>vic0nt</t>
   </si>
   <si>
-    <t>0 ч. 54 мин. 3 сек.</t>
+    <t>0 ч. 54 мин. 03 сек.</t>
   </si>
   <si>
     <t>ehh</t>
@@ -3119,7 +3119,7 @@
     <t>Morbid_Angel</t>
   </si>
   <si>
-    <t>1 ч. 3 мин. 5 сек.</t>
+    <t>1 ч. 03 мин. 05 сек.</t>
   </si>
   <si>
     <t>Kir_V</t>
@@ -3131,7 +3131,7 @@
     <t>Кот_Черныш</t>
   </si>
   <si>
-    <t>8 ч. 2 мин. 14 сек.</t>
+    <t>8 ч. 02 мин. 14 сек.</t>
   </si>
   <si>
     <t>409–413</t>
@@ -3152,7 +3152,7 @@
     <t>Chame</t>
   </si>
   <si>
-    <t>2 ч. 1 мин. 49 сек.</t>
+    <t>2 ч. 01 мин. 49 сек.</t>
   </si>
   <si>
     <t>wxkult</t>
@@ -3164,7 +3164,7 @@
     <t>_Jack_</t>
   </si>
   <si>
-    <t>3 ч. 55 мин. 8 сек.</t>
+    <t>3 ч. 55 мин. 08 сек.</t>
   </si>
   <si>
     <t>414–417</t>
@@ -3179,13 +3179,13 @@
     <t>SmartParkour</t>
   </si>
   <si>
-    <t>0 ч. 54 мин. 2 сек.</t>
+    <t>0 ч. 54 мин. 02 сек.</t>
   </si>
   <si>
     <t>mishlen79</t>
   </si>
   <si>
-    <t>1 ч. 5 мин. 26 сек.</t>
+    <t>1 ч. 05 мин. 26 сек.</t>
   </si>
   <si>
     <t>vezderegit</t>
@@ -3206,7 +3206,7 @@
     <t>SquirrelFox</t>
   </si>
   <si>
-    <t>1 ч. 1 мин. 35 сек.</t>
+    <t>1 ч. 01 мин. 35 сек.</t>
   </si>
   <si>
     <t>Лелюгри</t>
@@ -3236,7 +3236,7 @@
     <t>supertux_038</t>
   </si>
   <si>
-    <t>1 ч. 0 мин. 9 сек.</t>
+    <t>1 ч. 00 мин. 09 сек.</t>
   </si>
   <si>
     <t>ТОМА-АТОМНАЯ</t>
@@ -3275,7 +3275,7 @@
     <t>Kml</t>
   </si>
   <si>
-    <t>2 ч. 58 мин. 6 сек.</t>
+    <t>2 ч. 58 мин. 06 сек.</t>
   </si>
   <si>
     <t>430–434</t>
@@ -3284,19 +3284,19 @@
     <t>biznesman</t>
   </si>
   <si>
-    <t>0 ч. 44 мин. 2 сек.</t>
+    <t>0 ч. 44 мин. 02 сек.</t>
   </si>
   <si>
     <t>Sesquipedalian</t>
   </si>
   <si>
-    <t>0 ч. 45 мин. 9 сек.</t>
+    <t>0 ч. 45 мин. 09 сек.</t>
   </si>
   <si>
     <t>Фаст</t>
   </si>
   <si>
-    <t>1 ч. 44 мин. 5 сек.</t>
+    <t>1 ч. 44 мин. 05 сек.</t>
   </si>
   <si>
     <t>Althea_Fullmoon</t>
@@ -3308,7 +3308,7 @@
     <t>moonwwwind</t>
   </si>
   <si>
-    <t>7 ч. 12 мин. 5 сек.</t>
+    <t>7 ч. 12 мин. 05 сек.</t>
   </si>
   <si>
     <t>435</t>
@@ -3326,13 +3326,13 @@
     <t>Slavik89</t>
   </si>
   <si>
-    <t>1 ч. 14 мин. 8 сек.</t>
+    <t>1 ч. 14 мин. 08 сек.</t>
   </si>
   <si>
     <t>Developer313</t>
   </si>
   <si>
-    <t>1 ч. 24 мин. 1 сек.</t>
+    <t>1 ч. 24 мин. 01 сек.</t>
   </si>
   <si>
     <t>Всего_хорошего</t>
@@ -3344,7 +3344,7 @@
     <t>manfies</t>
   </si>
   <si>
-    <t>1 ч. 3 мин. 7 сек.</t>
+    <t>1 ч. 03 мин. 07 сек.</t>
   </si>
   <si>
     <t>SlyBeetle</t>
@@ -3386,7 +3386,7 @@
     <t>rseniy3</t>
   </si>
   <si>
-    <t>1 ч. 9 мин. 6 сек.</t>
+    <t>1 ч. 09 мин. 06 сек.</t>
   </si>
   <si>
     <t>446–447</t>
@@ -3395,7 +3395,7 @@
     <t>Импульс</t>
   </si>
   <si>
-    <t>1 ч. 0 мин. 0 сек.</t>
+    <t>1 ч. 00 мин. 00 сек.</t>
   </si>
   <si>
     <t>fuel_injection</t>
@@ -3416,7 +3416,7 @@
     <t>POSIX</t>
   </si>
   <si>
-    <t>9 ч. 3 мин. 7 сек.</t>
+    <t>9 ч. 03 мин. 07 сек.</t>
   </si>
   <si>
     <t>450–454</t>
@@ -3449,7 +3449,7 @@
     <t>Levileipheimer</t>
   </si>
   <si>
-    <t>3 ч. 52 мин. 4 сек.</t>
+    <t>3 ч. 52 мин. 04 сек.</t>
   </si>
   <si>
     <t>455–457</t>
@@ -3458,13 +3458,13 @@
     <t>Selica</t>
   </si>
   <si>
-    <t>1 ч. 2 мин. 48 сек.</t>
+    <t>1 ч. 02 мин. 48 сек.</t>
   </si>
   <si>
     <t>dvimster</t>
   </si>
   <si>
-    <t>1 ч. 20 мин. 8 сек.</t>
+    <t>1 ч. 20 мин. 08 сек.</t>
   </si>
   <si>
     <t>Vadim_K</t>
@@ -3506,7 +3506,7 @@
     <t>Symbo</t>
   </si>
   <si>
-    <t>0 ч. 32 мин. 4 сек.</t>
+    <t>0 ч. 32 мин. 04 сек.</t>
   </si>
   <si>
     <t>radambas</t>
@@ -3539,7 +3539,7 @@
     <t>DvoraQwer</t>
   </si>
   <si>
-    <t>2 ч. 1 мин. 8 сек.</t>
+    <t>2 ч. 01 мин. 08 сек.</t>
   </si>
   <si>
     <t>468–471</t>
@@ -3587,7 +3587,7 @@
     <t>lep</t>
   </si>
   <si>
-    <t>2 ч. 7 мин. 13 сек.</t>
+    <t>2 ч. 07 мин. 13 сек.</t>
   </si>
   <si>
     <t>north_air</t>
@@ -3602,13 +3602,13 @@
     <t>balanenko</t>
   </si>
   <si>
-    <t>1 ч. 8 мин. 53 сек.</t>
+    <t>1 ч. 08 мин. 53 сек.</t>
   </si>
   <si>
     <t>mixalezhnev</t>
   </si>
   <si>
-    <t>1 ч. 3 мин. 29 сек.</t>
+    <t>1 ч. 03 мин. 29 сек.</t>
   </si>
   <si>
     <t>Кибертаксист</t>
@@ -3635,7 +3635,7 @@
     <t>coolgrave</t>
   </si>
   <si>
-    <t>1 ч. 36 мин. 1 сек.</t>
+    <t>1 ч. 36 мин. 01 сек.</t>
   </si>
   <si>
     <t>Spetznaz</t>
@@ -3656,7 +3656,7 @@
     <t>KikiJiki85</t>
   </si>
   <si>
-    <t>2 ч. 5 мин. 17 сек.</t>
+    <t>2 ч. 05 мин. 17 сек.</t>
   </si>
   <si>
     <t>BogdanK</t>
@@ -3677,7 +3677,7 @@
     <t>KOSTYA410</t>
   </si>
   <si>
-    <t>1 ч. 7 мин. 44 сек.</t>
+    <t>1 ч. 07 мин. 44 сек.</t>
   </si>
   <si>
     <t>488–489</t>
@@ -3692,7 +3692,7 @@
     <t>smbody</t>
   </si>
   <si>
-    <t>3 ч. 8 мин. 27 сек.</t>
+    <t>3 ч. 08 мин. 27 сек.</t>
   </si>
   <si>
     <t>490</t>
@@ -3719,13 +3719,13 @@
     <t>bwp</t>
   </si>
   <si>
-    <t>1 ч. 4 мин. 52 сек.</t>
+    <t>1 ч. 04 мин. 52 сек.</t>
   </si>
   <si>
     <t>Стартуем</t>
   </si>
   <si>
-    <t>3 ч. 46 мин. 2 сек.</t>
+    <t>3 ч. 46 мин. 02 сек.</t>
   </si>
   <si>
     <t>495–496</t>
@@ -3746,7 +3746,7 @@
     <t>S0meOne</t>
   </si>
   <si>
-    <t>1 ч. 0 мин. 28 сек.</t>
+    <t>1 ч. 00 мин. 28 сек.</t>
   </si>
   <si>
     <t>Анна_Банановна</t>
@@ -3776,7 +3776,7 @@
     <t>Feliks_Smetana</t>
   </si>
   <si>
-    <t>21 ч. 8 мин. 10 сек.</t>
+    <t>21 ч. 08 мин. 10 сек.</t>
   </si>
   <si>
     <t>503–507</t>
@@ -3797,13 +3797,13 @@
     <t>chievo</t>
   </si>
   <si>
-    <t>3 ч. 5 мин. 20 сек.</t>
+    <t>3 ч. 05 мин. 20 сек.</t>
   </si>
   <si>
     <t>akaJackson</t>
   </si>
   <si>
-    <t>7 ч. 39 мин. 5 сек.</t>
+    <t>7 ч. 39 мин. 05 сек.</t>
   </si>
   <si>
     <t>ofirinka</t>
@@ -3878,7 +3878,7 @@
     <t>EclipseJDK</t>
   </si>
   <si>
-    <t>1 ч. 33 мин. 6 сек.</t>
+    <t>1 ч. 33 мин. 06 сек.</t>
   </si>
   <si>
     <t>ivchak</t>
@@ -3929,13 +3929,13 @@
     <t>eowyn_eorling</t>
   </si>
   <si>
-    <t>1 ч. 21 мин. 7 сек.</t>
+    <t>1 ч. 21 мин. 07 сек.</t>
   </si>
   <si>
     <t>dertru</t>
   </si>
   <si>
-    <t>4 ч. 34 мин. 9 сек.</t>
+    <t>4 ч. 34 мин. 09 сек.</t>
   </si>
   <si>
     <t>heavy_ezh</t>
@@ -3977,7 +3977,7 @@
     <t>IvanProskura</t>
   </si>
   <si>
-    <t>5 ч. 14 мин. 5 сек.</t>
+    <t>5 ч. 14 мин. 05 сек.</t>
   </si>
   <si>
     <t>533–535</t>
@@ -3998,7 +3998,7 @@
     <t>Декарт</t>
   </si>
   <si>
-    <t>3 ч. 44 мин. 0 сек.</t>
+    <t>3 ч. 44 мин. 00 сек.</t>
   </si>
   <si>
     <t>536–539</t>
@@ -4061,7 +4061,7 @@
     <t>Feshchenko</t>
   </si>
   <si>
-    <t>1 ч. 14 мин. 2 сек.</t>
+    <t>1 ч. 14 мин. 02 сек.</t>
   </si>
   <si>
     <t>shicotus</t>
@@ -4073,7 +4073,7 @@
     <t>-insOMnia-</t>
   </si>
   <si>
-    <t>1 ч. 59 мин. 0 сек.</t>
+    <t>1 ч. 59 мин. 00 сек.</t>
   </si>
   <si>
     <t>Waleria</t>
@@ -4097,7 +4097,7 @@
     <t>JohnStone</t>
   </si>
   <si>
-    <t>17 ч. 1 мин. 17 сек.</t>
+    <t>17 ч. 01 мин. 17 сек.</t>
   </si>
   <si>
     <t>551–553</t>
@@ -4106,7 +4106,7 @@
     <t>Lena19</t>
   </si>
   <si>
-    <t>0 ч. 44 мин. 1 сек.</t>
+    <t>0 ч. 44 мин. 01 сек.</t>
   </si>
   <si>
     <t>LekcRg</t>
@@ -4127,13 +4127,13 @@
     <t>kulinich</t>
   </si>
   <si>
-    <t>0 ч. 42 мин. 5 сек.</t>
+    <t>0 ч. 42 мин. 05 сек.</t>
   </si>
   <si>
     <t>Пани_Тыковка</t>
   </si>
   <si>
-    <t>0 ч. 51 мин. 9 сек.</t>
+    <t>0 ч. 51 мин. 09 сек.</t>
   </si>
   <si>
     <t>Драндулет</t>
@@ -4187,7 +4187,7 @@
     <t>Alexanter-Its</t>
   </si>
   <si>
-    <t>0 ч. 46 мин. 2 сек.</t>
+    <t>0 ч. 46 мин. 02 сек.</t>
   </si>
   <si>
     <t>Sensimiliya</t>
@@ -4208,7 +4208,7 @@
     <t>730sm</t>
   </si>
   <si>
-    <t>2 ч. 20 мин. 0 сек.</t>
+    <t>2 ч. 20 мин. 00 сек.</t>
   </si>
   <si>
     <t>567</t>
@@ -4226,7 +4226,7 @@
     <t>Leshiy239</t>
   </si>
   <si>
-    <t>1 ч. 0 мин. 48 сек.</t>
+    <t>1 ч. 00 мин. 48 сек.</t>
   </si>
   <si>
     <t>Irina_25</t>
@@ -4268,7 +4268,7 @@
     <t>akaSStalkALEX</t>
   </si>
   <si>
-    <t>1 ч. 3 мин. 31 сек.</t>
+    <t>1 ч. 03 мин. 31 сек.</t>
   </si>
   <si>
     <t>575–577</t>
@@ -4277,7 +4277,7 @@
     <t>Misprinter</t>
   </si>
   <si>
-    <t>1 ч. 15 мин. 8 сек.</t>
+    <t>1 ч. 15 мин. 08 сек.</t>
   </si>
   <si>
     <t>vlad992</t>
@@ -4316,13 +4316,13 @@
     <t>_Ayrat_</t>
   </si>
   <si>
-    <t>1 ч. 40 мин. 8 сек.</t>
+    <t>1 ч. 40 мин. 08 сек.</t>
   </si>
   <si>
     <t>ZUN</t>
   </si>
   <si>
-    <t>5 ч. 27 мин. 1 сек.</t>
+    <t>5 ч. 27 мин. 01 сек.</t>
   </si>
   <si>
     <t>583–585</t>
@@ -4337,13 +4337,13 @@
     <t>andreyusamo</t>
   </si>
   <si>
-    <t>0 ч. 36 мин. 7 сек.</t>
+    <t>0 ч. 36 мин. 07 сек.</t>
   </si>
   <si>
     <t>exektc</t>
   </si>
   <si>
-    <t>7 ч. 1 мин. 39 сек.</t>
+    <t>7 ч. 01 мин. 39 сек.</t>
   </si>
   <si>
     <t>586</t>
@@ -4352,7 +4352,7 @@
     <t>nadia_myronuk</t>
   </si>
   <si>
-    <t>3 ч. 8 мин. 9 сек.</t>
+    <t>3 ч. 08 мин. 09 сек.</t>
   </si>
   <si>
     <t>587–588</t>
@@ -4397,7 +4397,7 @@
     <t>felicia_</t>
   </si>
   <si>
-    <t>1 ч. 6 мин. 28 сек.</t>
+    <t>1 ч. 06 мин. 28 сек.</t>
   </si>
   <si>
     <t>Syritchenko</t>
@@ -4433,13 +4433,13 @@
     <t>Эвольвента</t>
   </si>
   <si>
-    <t>0 ч. 54 мин. 6 сек.</t>
+    <t>0 ч. 54 мин. 06 сек.</t>
   </si>
   <si>
     <t>uniko</t>
   </si>
   <si>
-    <t>1 ч. 11 мин. 7 сек.</t>
+    <t>1 ч. 11 мин. 07 сек.</t>
   </si>
   <si>
     <t>599–601</t>
@@ -4448,7 +4448,7 @@
     <t>Vesna2011</t>
   </si>
   <si>
-    <t>1 ч. 4 мин. 31 сек.</t>
+    <t>1 ч. 04 мин. 31 сек.</t>
   </si>
   <si>
     <t>Соточка</t>
@@ -4475,7 +4475,7 @@
     <t>userbit</t>
   </si>
   <si>
-    <t>1 ч. 5 мин. 29 сек.</t>
+    <t>1 ч. 05 мин. 29 сек.</t>
   </si>
   <si>
     <t>martast</t>
@@ -4520,13 +4520,13 @@
     <t>Русский_топор</t>
   </si>
   <si>
-    <t>0 ч. 39 мин. 3 сек.</t>
+    <t>0 ч. 39 мин. 03 сек.</t>
   </si>
   <si>
     <t>strakhov94</t>
   </si>
   <si>
-    <t>1 ч. 2 мин. 49 сек.</t>
+    <t>1 ч. 02 мин. 49 сек.</t>
   </si>
   <si>
     <t>qwertyasdfg</t>
@@ -4559,7 +4559,7 @@
     <t>tinto</t>
   </si>
   <si>
-    <t>2 ч. 19 мин. 8 сек.</t>
+    <t>2 ч. 19 мин. 08 сек.</t>
   </si>
   <si>
     <t>616–617</t>
@@ -4574,7 +4574,7 @@
     <t>denisov7</t>
   </si>
   <si>
-    <t>3 ч. 6 мин. 43 сек.</t>
+    <t>3 ч. 06 мин. 43 сек.</t>
   </si>
   <si>
     <t>618–622</t>
@@ -4607,7 +4607,7 @@
     <t>valula</t>
   </si>
   <si>
-    <t>20 ч. 1 мин. 5 сек.</t>
+    <t>20 ч. 01 мин. 05 сек.</t>
   </si>
   <si>
     <t>623–625</t>
@@ -4616,13 +4616,13 @@
     <t>visoko</t>
   </si>
   <si>
-    <t>1 ч. 1 мин. 49 сек.</t>
+    <t>1 ч. 01 мин. 49 сек.</t>
   </si>
   <si>
     <t>beethoven</t>
   </si>
   <si>
-    <t>1 ч. 1 мин. 29 сек.</t>
+    <t>1 ч. 01 мин. 29 сек.</t>
   </si>
   <si>
     <t>Навальный</t>
@@ -4637,7 +4637,7 @@
     <t>fedind</t>
   </si>
   <si>
-    <t>0 ч. 36 мин. 4 сек.</t>
+    <t>0 ч. 36 мин. 04 сек.</t>
   </si>
   <si>
     <t>Mirtum</t>
@@ -4691,19 +4691,19 @@
     <t>Alington</t>
   </si>
   <si>
-    <t>0 ч. 46 мин. 3 сек.</t>
+    <t>0 ч. 46 мин. 03 сек.</t>
   </si>
   <si>
     <t>osipetka</t>
   </si>
   <si>
-    <t>1 ч. 11 мин. 0 сек.</t>
+    <t>1 ч. 11 мин. 00 сек.</t>
   </si>
   <si>
     <t>vladdotac</t>
   </si>
   <si>
-    <t>1 ч. 7 мин. 10 сек.</t>
+    <t>1 ч. 07 мин. 10 сек.</t>
   </si>
   <si>
     <t>Shena</t>
@@ -4733,7 +4733,7 @@
     <t>Newaton</t>
   </si>
   <si>
-    <t>1 ч. 31 мин. 0 сек.</t>
+    <t>1 ч. 31 мин. 00 сек.</t>
   </si>
   <si>
     <t>Mugvor</t>
@@ -4784,19 +4784,19 @@
     <t>драконДьявола</t>
   </si>
   <si>
-    <t>1 ч. 4 мин. 7 сек.</t>
+    <t>1 ч. 04 мин. 07 сек.</t>
   </si>
   <si>
     <t>alanen</t>
   </si>
   <si>
-    <t>1 ч. 9 мин. 53 сек.</t>
+    <t>1 ч. 09 мин. 53 сек.</t>
   </si>
   <si>
     <t>fedyagor</t>
   </si>
   <si>
-    <t>2 ч. 0 мин. 5 сек.</t>
+    <t>2 ч. 00 мин. 05 сек.</t>
   </si>
   <si>
     <t>НиколайГесс</t>
@@ -4841,7 +4841,7 @@
     <t>yescast</t>
   </si>
   <si>
-    <t>1 ч. 0 мин. 37 сек.</t>
+    <t>1 ч. 00 мин. 37 сек.</t>
   </si>
   <si>
     <t>second</t>
@@ -4853,7 +4853,7 @@
     <t>iBumble</t>
   </si>
   <si>
-    <t>4 ч. 3 мин. 26 сек.</t>
+    <t>4 ч. 03 мин. 26 сек.</t>
   </si>
   <si>
     <t>659</t>
@@ -4877,7 +4877,7 @@
     <t>romashe</t>
   </si>
   <si>
-    <t>1 ч. 4 мин. 39 сек.</t>
+    <t>1 ч. 04 мин. 39 сек.</t>
   </si>
   <si>
     <t>662–664</t>
@@ -4964,7 +4964,7 @@
     <t>Zerstoren</t>
   </si>
   <si>
-    <t>2 ч. 19 мин. 4 сек.</t>
+    <t>2 ч. 19 мин. 04 сек.</t>
   </si>
   <si>
     <t>674–676</t>
@@ -4973,7 +4973,7 @@
     <t>kasiveyser</t>
   </si>
   <si>
-    <t>1 ч. 9 мин. 23 сек.</t>
+    <t>1 ч. 09 мин. 23 сек.</t>
   </si>
   <si>
     <t>oleonik</t>
@@ -5003,13 +5003,13 @@
     <t>kxinekton</t>
   </si>
   <si>
-    <t>1 ч. 4 мин. 0 сек.</t>
+    <t>1 ч. 04 мин. 00 сек.</t>
   </si>
   <si>
     <t>Klume</t>
   </si>
   <si>
-    <t>2 ч. 7 мин. 29 сек.</t>
+    <t>2 ч. 07 мин. 29 сек.</t>
   </si>
   <si>
     <t>roya3000</t>
@@ -5042,7 +5042,7 @@
     <t>yurgen55</t>
   </si>
   <si>
-    <t>10 ч. 30 мин. 4 сек.</t>
+    <t>10 ч. 30 мин. 04 сек.</t>
   </si>
   <si>
     <t>685–689</t>
@@ -5051,13 +5051,13 @@
     <t>HudsonHorny</t>
   </si>
   <si>
-    <t>0 ч. 43 мин. 0 сек.</t>
+    <t>0 ч. 43 мин. 00 сек.</t>
   </si>
   <si>
     <t>odto11</t>
   </si>
   <si>
-    <t>0 ч. 53 мин. 7 сек.</t>
+    <t>0 ч. 53 мин. 07 сек.</t>
   </si>
   <si>
     <t>Detan</t>
@@ -5069,13 +5069,13 @@
     <t>Анетточка</t>
   </si>
   <si>
-    <t>2 ч. 44 мин. 9 сек.</t>
+    <t>2 ч. 44 мин. 09 сек.</t>
   </si>
   <si>
     <t>learnToType</t>
   </si>
   <si>
-    <t>13 ч. 1 мин. 10 сек.</t>
+    <t>13 ч. 01 мин. 10 сек.</t>
   </si>
   <si>
     <t>690–691</t>
@@ -5090,7 +5090,7 @@
     <t>-santiago-</t>
   </si>
   <si>
-    <t>3 ч. 6 мин. 6 сек.</t>
+    <t>3 ч. 06 мин. 06 сек.</t>
   </si>
   <si>
     <t>692–694</t>
@@ -5105,7 +5105,7 @@
     <t>KindOf</t>
   </si>
   <si>
-    <t>0 ч. 49 мин. 7 сек.</t>
+    <t>0 ч. 49 мин. 07 сек.</t>
   </si>
   <si>
     <t>slelaron</t>
@@ -5135,13 +5135,13 @@
     <t>puma3033</t>
   </si>
   <si>
-    <t>1 ч. 5 мин. 4 сек.</t>
+    <t>1 ч. 05 мин. 04 сек.</t>
   </si>
   <si>
     <t>Voldik</t>
   </si>
   <si>
-    <t>7 ч. 29 мин. 0 сек.</t>
+    <t>7 ч. 29 мин. 00 сек.</t>
   </si>
   <si>
     <t>699–704</t>
@@ -5168,13 +5168,13 @@
     <t>maikttt</t>
   </si>
   <si>
-    <t>2 ч. 33 мин. 4 сек.</t>
+    <t>2 ч. 33 мин. 04 сек.</t>
   </si>
   <si>
     <t>отлезь_вова</t>
   </si>
   <si>
-    <t>5 ч. 7 мин. 47 сек.</t>
+    <t>5 ч. 07 мин. 47 сек.</t>
   </si>
   <si>
     <t>Andy333</t>
@@ -5192,7 +5192,7 @@
     <t>Leolex</t>
   </si>
   <si>
-    <t>1 ч. 22 мин. 0 сек.</t>
+    <t>1 ч. 22 мин. 00 сек.</t>
   </si>
   <si>
     <t>darkgame0</t>
@@ -5216,7 +5216,7 @@
     <t>CyrCyr</t>
   </si>
   <si>
-    <t>2 ч. 5 мин. 4 сек.</t>
+    <t>2 ч. 05 мин. 04 сек.</t>
   </si>
   <si>
     <t>Antonio_Zts</t>
@@ -5237,7 +5237,7 @@
     <t>8788</t>
   </si>
   <si>
-    <t>4 ч. 5 мин. 41 сек.</t>
+    <t>4 ч. 05 мин. 41 сек.</t>
   </si>
   <si>
     <t>714–715</t>
@@ -5252,7 +5252,7 @@
     <t>CTuKEP</t>
   </si>
   <si>
-    <t>1 ч. 56 мин. 2 сек.</t>
+    <t>1 ч. 56 мин. 02 сек.</t>
   </si>
   <si>
     <t>716</t>
@@ -5276,7 +5276,7 @@
     <t>Meteora277</t>
   </si>
   <si>
-    <t>1 ч. 3 мин. 42 сек.</t>
+    <t>1 ч. 03 мин. 42 сек.</t>
   </si>
   <si>
     <t>Mad_Falcon</t>
@@ -5300,7 +5300,7 @@
     <t>Рустамко</t>
   </si>
   <si>
-    <t>2 ч. 2 мин. 40 сек.</t>
+    <t>2 ч. 02 мин. 40 сек.</t>
   </si>
   <si>
     <t>HappyHardcore</t>
@@ -5354,7 +5354,7 @@
     <t>ntfs</t>
   </si>
   <si>
-    <t>1 ч. 2 мин. 30 сек.</t>
+    <t>1 ч. 02 мин. 30 сек.</t>
   </si>
   <si>
     <t>arokoko</t>
@@ -5390,7 +5390,7 @@
     <t>ShavgaStas</t>
   </si>
   <si>
-    <t>1 ч. 43 мин. 4 сек.</t>
+    <t>1 ч. 43 мин. 04 сек.</t>
   </si>
   <si>
     <t>ArtHare</t>
@@ -5423,7 +5423,7 @@
     <t>Engi</t>
   </si>
   <si>
-    <t>1 ч. 17 мин. 2 сек.</t>
+    <t>1 ч. 17 мин. 02 сек.</t>
   </si>
   <si>
     <t>panteraD</t>
@@ -5435,7 +5435,7 @@
     <t>vl7</t>
   </si>
   <si>
-    <t>12 ч. 8 мин. 37 сек.</t>
+    <t>12 ч. 08 мин. 37 сек.</t>
   </si>
   <si>
     <t>742–743</t>
@@ -5444,7 +5444,7 @@
     <t>xxl11</t>
   </si>
   <si>
-    <t>1 ч. 5 мин. 31 сек.</t>
+    <t>1 ч. 05 мин. 31 сек.</t>
   </si>
   <si>
     <t>Shivaki</t>
@@ -5459,13 +5459,13 @@
     <t>potykk</t>
   </si>
   <si>
-    <t>0 ч. 54 мин. 5 сек.</t>
+    <t>0 ч. 54 мин. 05 сек.</t>
   </si>
   <si>
     <t>Dany</t>
   </si>
   <si>
-    <t>1 ч. 1 мин. 50 сек.</t>
+    <t>1 ч. 01 мин. 50 сек.</t>
   </si>
   <si>
     <t>Sofi15050888</t>
@@ -5498,7 +5498,7 @@
     <t>самурай_47_</t>
   </si>
   <si>
-    <t>2 ч. 32 мин. 4 сек.</t>
+    <t>2 ч. 32 мин. 04 сек.</t>
   </si>
   <si>
     <t>tomplier</t>
@@ -5513,13 +5513,13 @@
     <t>vrv1993</t>
   </si>
   <si>
-    <t>0 ч. 46 мин. 9 сек.</t>
+    <t>0 ч. 46 мин. 09 сек.</t>
   </si>
   <si>
     <t>gevis</t>
   </si>
   <si>
-    <t>1 ч. 24 мин. 0 сек.</t>
+    <t>1 ч. 24 мин. 00 сек.</t>
   </si>
   <si>
     <t>Shomka5</t>
@@ -5588,19 +5588,19 @@
     <t>Aus</t>
   </si>
   <si>
-    <t>1 ч. 21 мин. 1 сек.</t>
+    <t>1 ч. 21 мин. 01 сек.</t>
   </si>
   <si>
     <t>qqaezz</t>
   </si>
   <si>
-    <t>3 ч. 5 мин. 40 сек.</t>
+    <t>3 ч. 05 мин. 40 сек.</t>
   </si>
   <si>
     <t>tfn3k</t>
   </si>
   <si>
-    <t>3 ч. 2 мин. 5 сек.</t>
+    <t>3 ч. 02 мин. 05 сек.</t>
   </si>
   <si>
     <t>766</t>
@@ -5609,7 +5609,7 @@
     <t>hangling</t>
   </si>
   <si>
-    <t>7 ч. 53 мин. 6 сек.</t>
+    <t>7 ч. 53 мин. 06 сек.</t>
   </si>
   <si>
     <t>767–770</t>
@@ -5618,7 +5618,7 @@
     <t>ГОЧА</t>
   </si>
   <si>
-    <t>2 ч. 26 мин. 1 сек.</t>
+    <t>2 ч. 26 мин. 01 сек.</t>
   </si>
   <si>
     <t>Гектор</t>
@@ -5636,7 +5636,7 @@
     <t>Asp1ro_</t>
   </si>
   <si>
-    <t>10 ч. 26 мин. 8 сек.</t>
+    <t>10 ч. 26 мин. 08 сек.</t>
   </si>
   <si>
     <t>771–772</t>
@@ -5669,7 +5669,7 @@
     <t>madk1nd</t>
   </si>
   <si>
-    <t>1 ч. 13 мин. 2 сек.</t>
+    <t>1 ч. 13 мин. 02 сек.</t>
   </si>
   <si>
     <t>-Жу-</t>
@@ -5690,7 +5690,7 @@
     <t>Мимо_Крокодил</t>
   </si>
   <si>
-    <t>1 ч. 4 мин. 24 сек.</t>
+    <t>1 ч. 04 мин. 24 сек.</t>
   </si>
   <si>
     <t>hamster2240</t>
@@ -5714,7 +5714,7 @@
     <t>masque_otrd</t>
   </si>
   <si>
-    <t>3 ч. 8 мин. 17 сек.</t>
+    <t>3 ч. 08 мин. 17 сек.</t>
   </si>
   <si>
     <t>dumb</t>
@@ -5762,7 +5762,7 @@
     <t>VladimirFvR</t>
   </si>
   <si>
-    <t>39 ч. 7 мин. 16 сек.</t>
+    <t>39 ч. 07 мин. 16 сек.</t>
   </si>
   <si>
     <t>790–794</t>
@@ -5771,7 +5771,7 @@
     <t>Argregor</t>
   </si>
   <si>
-    <t>1 ч. 11 мин. 2 сек.</t>
+    <t>1 ч. 11 мин. 02 сек.</t>
   </si>
   <si>
     <t>Taypun</t>
@@ -5783,7 +5783,7 @@
     <t>флибустьер</t>
   </si>
   <si>
-    <t>2 ч. 46 мин. 6 сек.</t>
+    <t>2 ч. 46 мин. 06 сек.</t>
   </si>
   <si>
     <t>Mister_Finka</t>
@@ -5795,7 +5795,7 @@
     <t>cybrg</t>
   </si>
   <si>
-    <t>3 ч. 0 мин. 28 сек.</t>
+    <t>3 ч. 00 мин. 28 сек.</t>
   </si>
   <si>
     <t>795</t>
@@ -5813,7 +5813,7 @@
     <t>chp0ks</t>
   </si>
   <si>
-    <t>0 ч. 59 мин. 3 сек.</t>
+    <t>0 ч. 59 мин. 03 сек.</t>
   </si>
   <si>
     <t>MoskovKazanova</t>
@@ -5831,7 +5831,7 @@
     <t>нуммулит</t>
   </si>
   <si>
-    <t>4 ч. 48 мин. 5 сек.</t>
+    <t>4 ч. 48 мин. 05 сек.</t>
   </si>
   <si>
     <t>800–802</t>
@@ -5840,7 +5840,7 @@
     <t>YE11OW</t>
   </si>
   <si>
-    <t>1 ч. 1 мин. 52 сек.</t>
+    <t>1 ч. 01 мин. 52 сек.</t>
   </si>
   <si>
     <t>ZverikK</t>
@@ -5888,7 +5888,7 @@
     <t>Mirion</t>
   </si>
   <si>
-    <t>4 ч. 59 мин. 4 сек.</t>
+    <t>4 ч. 59 мин. 04 сек.</t>
   </si>
   <si>
     <t>808–811</t>
@@ -5897,19 +5897,19 @@
     <t>gluckss2</t>
   </si>
   <si>
-    <t>1 ч. 23 мин. 3 сек.</t>
+    <t>1 ч. 23 мин. 03 сек.</t>
   </si>
   <si>
     <t>Странник</t>
   </si>
   <si>
-    <t>2 ч. 9 мин. 19 сек.</t>
+    <t>2 ч. 09 мин. 19 сек.</t>
   </si>
   <si>
     <t>inteltone</t>
   </si>
   <si>
-    <t>11 ч. 30 мин. 3 сек.</t>
+    <t>11 ч. 30 мин. 03 сек.</t>
   </si>
   <si>
     <t>msiWind90</t>
@@ -5936,7 +5936,7 @@
     <t>Хуля</t>
   </si>
   <si>
-    <t>10 ч. 4 мин. 43 сек.</t>
+    <t>10 ч. 04 мин. 43 сек.</t>
   </si>
   <si>
     <t>Stooge</t>
@@ -5963,7 +5963,7 @@
     <t>veron9399</t>
   </si>
   <si>
-    <t>1 ч. 55 мин. 1 сек.</t>
+    <t>1 ч. 55 мин. 01 сек.</t>
   </si>
   <si>
     <t>819–826</t>
@@ -5984,7 +5984,7 @@
     <t>Wasily</t>
   </si>
   <si>
-    <t>1 ч. 0 мин. 16 сек.</t>
+    <t>1 ч. 00 мин. 16 сек.</t>
   </si>
   <si>
     <t>kaskadkaskadov</t>
@@ -6008,7 +6008,7 @@
     <t>Eyeless</t>
   </si>
   <si>
-    <t>2 ч. 30 мин. 0 сек.</t>
+    <t>2 ч. 30 мин. 00 сек.</t>
   </si>
   <si>
     <t>Agen</t>
@@ -6074,7 +6074,7 @@
     <t>murtag</t>
   </si>
   <si>
-    <t>5 ч. 4 мин. 1 сек.</t>
+    <t>5 ч. 04 мин. 01 сек.</t>
   </si>
   <si>
     <t>836</t>
@@ -6101,7 +6101,7 @@
     <t>Миша-Буденновск</t>
   </si>
   <si>
-    <t>1 ч. 1 мин. 57 сек.</t>
+    <t>1 ч. 01 мин. 57 сек.</t>
   </si>
   <si>
     <t>milyasow</t>
@@ -6113,13 +6113,13 @@
     <t>kosal</t>
   </si>
   <si>
-    <t>1 ч. 41 мин. 5 сек.</t>
+    <t>1 ч. 41 мин. 05 сек.</t>
   </si>
   <si>
     <t>NK7</t>
   </si>
   <si>
-    <t>2 ч. 5 мин. 52 сек.</t>
+    <t>2 ч. 05 мин. 52 сек.</t>
   </si>
   <si>
     <t>NodeJS</t>
@@ -6149,13 +6149,13 @@
     <t>getsomeweed</t>
   </si>
   <si>
-    <t>0 ч. 56 мин. 9 сек.</t>
+    <t>0 ч. 56 мин. 09 сек.</t>
   </si>
   <si>
     <t>Кнопкомет</t>
   </si>
   <si>
-    <t>1 ч. 5 мин. 58 сек.</t>
+    <t>1 ч. 05 мин. 58 сек.</t>
   </si>
   <si>
     <t>Igem</t>
@@ -6167,13 +6167,13 @@
     <t>nick1m</t>
   </si>
   <si>
-    <t>5 ч. 6 мин. 8 сек.</t>
+    <t>5 ч. 06 мин. 08 сек.</t>
   </si>
   <si>
     <t>f0rtuna</t>
   </si>
   <si>
-    <t>8 ч. 2 мин. 21 сек.</t>
+    <t>8 ч. 02 мин. 21 сек.</t>
   </si>
   <si>
     <t>bash2b</t>
@@ -6188,7 +6188,7 @@
     <t>drago1233</t>
   </si>
   <si>
-    <t>1 ч. 3 мин. 44 сек.</t>
+    <t>1 ч. 03 мин. 44 сек.</t>
   </si>
   <si>
     <t>vladyan</t>
@@ -6221,7 +6221,7 @@
     <t>AllMo</t>
   </si>
   <si>
-    <t>1 ч. 0 мин. 1 сек.</t>
+    <t>1 ч. 00 мин. 01 сек.</t>
   </si>
   <si>
     <t>IxC999</t>
@@ -6293,7 +6293,7 @@
     <t>vlad200</t>
   </si>
   <si>
-    <t>133 ч. 29 мин. 5 сек.</t>
+    <t>133 ч. 29 мин. 05 сек.</t>
   </si>
   <si>
     <t>867–868</t>
@@ -6308,7 +6308,7 @@
     <t>ОКейка</t>
   </si>
   <si>
-    <t>1 ч. 6 мин. 23 сек.</t>
+    <t>1 ч. 06 мин. 23 сек.</t>
   </si>
   <si>
     <t>869–872</t>
@@ -6323,7 +6323,7 @@
     <t>Going</t>
   </si>
   <si>
-    <t>3 ч. 33 мин. 5 сек.</t>
+    <t>3 ч. 33 мин. 05 сек.</t>
   </si>
   <si>
     <t>gonwikklavo</t>
@@ -6383,7 +6383,7 @@
     <t>Ladimir</t>
   </si>
   <si>
-    <t>1 ч. 58 мин. 6 сек.</t>
+    <t>1 ч. 58 мин. 06 сек.</t>
   </si>
   <si>
     <t>zh-tanchik</t>
@@ -6398,7 +6398,7 @@
     <t>JohnDoe12</t>
   </si>
   <si>
-    <t>0 ч. 59 мин. 8 сек.</t>
+    <t>0 ч. 59 мин. 08 сек.</t>
   </si>
   <si>
     <t>dns1337</t>
@@ -6410,7 +6410,7 @@
     <t>sbhx</t>
   </si>
   <si>
-    <t>2 ч. 0 мин. 32 сек.</t>
+    <t>2 ч. 00 мин. 32 сек.</t>
   </si>
   <si>
     <t>free111</t>
@@ -6425,19 +6425,19 @@
     <t>alexandr-ftf</t>
   </si>
   <si>
-    <t>1 ч. 20 мин. 1 сек.</t>
+    <t>1 ч. 20 мин. 01 сек.</t>
   </si>
   <si>
     <t>Anun</t>
   </si>
   <si>
-    <t>1 ч. 58 мин. 5 сек.</t>
+    <t>1 ч. 58 мин. 05 сек.</t>
   </si>
   <si>
     <t>Аурика</t>
   </si>
   <si>
-    <t>5 ч. 53 мин. 2 сек.</t>
+    <t>5 ч. 53 мин. 02 сек.</t>
   </si>
   <si>
     <t>887</t>
@@ -6446,7 +6446,7 @@
     <t>Alhimik_ua</t>
   </si>
   <si>
-    <t>4 ч. 2 мин. 32 сек.</t>
+    <t>4 ч. 02 мин. 32 сек.</t>
   </si>
   <si>
     <t>888–891</t>
@@ -6455,13 +6455,13 @@
     <t>Kentan</t>
   </si>
   <si>
-    <t>1 ч. 0 мин. 45 сек.</t>
+    <t>1 ч. 00 мин. 45 сек.</t>
   </si>
   <si>
     <t>Vi2GaN</t>
   </si>
   <si>
-    <t>2 ч. 4 мин. 47 сек.</t>
+    <t>2 ч. 04 мин. 47 сек.</t>
   </si>
   <si>
     <t>Lamiya</t>
@@ -6506,7 +6506,7 @@
     <t>aliwagner</t>
   </si>
   <si>
-    <t>1 ч. 40 мин. 4 сек.</t>
+    <t>1 ч. 40 мин. 04 сек.</t>
   </si>
   <si>
     <t>9999999999</t>
@@ -6542,7 +6542,7 @@
     <t>TARDIS</t>
   </si>
   <si>
-    <t>3 ч. 2 мин. 49 сек.</t>
+    <t>3 ч. 02 мин. 49 сек.</t>
   </si>
   <si>
     <t>901</t>
@@ -6569,7 +6569,7 @@
     <t>barmaglot</t>
   </si>
   <si>
-    <t>10 ч. 57 мин. 4 сек.</t>
+    <t>10 ч. 57 мин. 04 сек.</t>
   </si>
   <si>
     <t>905–906</t>
@@ -6578,13 +6578,13 @@
     <t>Alkhor</t>
   </si>
   <si>
-    <t>1 ч. 9 мин. 35 сек.</t>
+    <t>1 ч. 09 мин. 35 сек.</t>
   </si>
   <si>
     <t>Nitro8715</t>
   </si>
   <si>
-    <t>4 ч. 7 мин. 41 сек.</t>
+    <t>4 ч. 07 мин. 41 сек.</t>
   </si>
   <si>
     <t>907–909</t>
@@ -6623,7 +6623,7 @@
     <t>prestor-jon</t>
   </si>
   <si>
-    <t>5 ч. 6 мин. 44 сек.</t>
+    <t>5 ч. 06 мин. 44 сек.</t>
   </si>
   <si>
     <t>913–915</t>
@@ -6638,7 +6638,7 @@
     <t>yapoehal</t>
   </si>
   <si>
-    <t>5 ч. 42 мин. 2 сек.</t>
+    <t>5 ч. 42 мин. 02 сек.</t>
   </si>
   <si>
     <t>Savitri</t>
@@ -6689,7 +6689,7 @@
     <t>_Влада_</t>
   </si>
   <si>
-    <t>1 ч. 28 мин. 1 сек.</t>
+    <t>1 ч. 28 мин. 01 сек.</t>
   </si>
   <si>
     <t>Wedgewood</t>
@@ -6701,7 +6701,7 @@
     <t>14bas14</t>
   </si>
   <si>
-    <t>3 ч. 5 мин. 42 сек.</t>
+    <t>3 ч. 05 мин. 42 сек.</t>
   </si>
   <si>
     <t>924</t>
@@ -6737,7 +6737,7 @@
     <t>Zephir</t>
   </si>
   <si>
-    <t>2 ч. 2 мин. 4 сек.</t>
+    <t>2 ч. 02 мин. 04 сек.</t>
   </si>
   <si>
     <t>MajoRicH</t>
@@ -6773,7 +6773,7 @@
     <t>violence23</t>
   </si>
   <si>
-    <t>1 ч. 4 мин. 12 сек.</t>
+    <t>1 ч. 04 мин. 12 сек.</t>
   </si>
   <si>
     <t>934–936</t>
@@ -6821,7 +6821,7 @@
     <t>JamesPenny</t>
   </si>
   <si>
-    <t>2 ч. 30 мин. 7 сек.</t>
+    <t>2 ч. 30 мин. 07 сек.</t>
   </si>
   <si>
     <t>941</t>
@@ -6830,7 +6830,7 @@
     <t>Stremer</t>
   </si>
   <si>
-    <t>1 ч. 46 мин. 1 сек.</t>
+    <t>1 ч. 46 мин. 01 сек.</t>
   </si>
   <si>
     <t>942–943</t>
@@ -6839,7 +6839,7 @@
     <t>manhunt7</t>
   </si>
   <si>
-    <t>1 ч. 10 мин. 8 сек.</t>
+    <t>1 ч. 10 мин. 08 сек.</t>
   </si>
   <si>
     <t>shadymarsh</t>
@@ -6899,7 +6899,7 @@
     <t>ivab</t>
   </si>
   <si>
-    <t>2 ч. 4 мин. 53 сек.</t>
+    <t>2 ч. 04 мин. 53 сек.</t>
   </si>
   <si>
     <t>jackodiamonds</t>
@@ -6911,7 +6911,7 @@
     <t>Red_Sky</t>
   </si>
   <si>
-    <t>4 ч. 2 мин. 21 сек.</t>
+    <t>4 ч. 02 мин. 21 сек.</t>
   </si>
   <si>
     <t>Barbed</t>
@@ -6926,13 +6926,13 @@
     <t>непотомуль</t>
   </si>
   <si>
-    <t>1 ч. 2 мин. 41 сек.</t>
+    <t>1 ч. 02 мин. 41 сек.</t>
   </si>
   <si>
     <t>ras2223car</t>
   </si>
   <si>
-    <t>1 ч. 40 мин. 9 сек.</t>
+    <t>1 ч. 40 мин. 09 сек.</t>
   </si>
   <si>
     <t>mr_ursu</t>
@@ -6944,7 +6944,7 @@
     <t>Ллисса</t>
   </si>
   <si>
-    <t>4 ч. 0 мин. 43 сек.</t>
+    <t>4 ч. 00 мин. 43 сек.</t>
   </si>
   <si>
     <t>958–960</t>
@@ -6953,13 +6953,13 @@
     <t>Drayn</t>
   </si>
   <si>
-    <t>1 ч. 5 мин. 19 сек.</t>
+    <t>1 ч. 05 мин. 19 сек.</t>
   </si>
   <si>
     <t>Мач</t>
   </si>
   <si>
-    <t>1 ч. 7 мин. 17 сек.</t>
+    <t>1 ч. 07 мин. 17 сек.</t>
   </si>
   <si>
     <t>Umunty</t>
@@ -7022,7 +7022,7 @@
     <t>nozim</t>
   </si>
   <si>
-    <t>2 ч. 26 мин. 6 сек.</t>
+    <t>2 ч. 26 мин. 06 сек.</t>
   </si>
   <si>
     <t>ssa774</t>
@@ -7037,13 +7037,13 @@
     <t>Brgl</t>
   </si>
   <si>
-    <t>0 ч. 58 мин. 6 сек.</t>
+    <t>0 ч. 58 мин. 06 сек.</t>
   </si>
   <si>
     <t>MilesH</t>
   </si>
   <si>
-    <t>2 ч. 8 мин. 46 сек.</t>
+    <t>2 ч. 08 мин. 46 сек.</t>
   </si>
   <si>
     <t>mariastime</t>
@@ -7064,7 +7064,7 @@
     <t>sovofeel</t>
   </si>
   <si>
-    <t>3 ч. 8 мин. 44 сек.</t>
+    <t>3 ч. 08 мин. 44 сек.</t>
   </si>
   <si>
     <t>975–976</t>
@@ -7088,7 +7088,7 @@
     <t>bronikkk</t>
   </si>
   <si>
-    <t>0 ч. 55 мин. 2 сек.</t>
+    <t>0 ч. 55 мин. 02 сек.</t>
   </si>
   <si>
     <t>Natalochka</t>
@@ -7115,13 +7115,13 @@
     <t>SamArKin</t>
   </si>
   <si>
-    <t>3 ч. 8 мин. 25 сек.</t>
+    <t>3 ч. 08 мин. 25 сек.</t>
   </si>
   <si>
     <t>tumanov2012</t>
   </si>
   <si>
-    <t>4 ч. 50 мин. 8 сек.</t>
+    <t>4 ч. 50 мин. 08 сек.</t>
   </si>
   <si>
     <t>983</t>
@@ -7157,7 +7157,7 @@
     <t>vitazik</t>
   </si>
   <si>
-    <t>2 ч. 57 мин. 3 сек.</t>
+    <t>2 ч. 57 мин. 03 сек.</t>
   </si>
   <si>
     <t>saneknovco</t>
@@ -7187,7 +7187,7 @@
     <t>LDNSB</t>
   </si>
   <si>
-    <t>1 ч. 1 мин. 34 сек.</t>
+    <t>1 ч. 01 мин. 34 сек.</t>
   </si>
   <si>
     <t>Arc_warden_kg1</t>
@@ -7307,7 +7307,7 @@
     <t>quantum_donchi</t>
   </si>
   <si>
-    <t>3 ч. 3 мин. 6 сек.</t>
+    <t>3 ч. 03 мин. 06 сек.</t>
   </si>
   <si>
     <t>1008</t>
@@ -7355,7 +7355,7 @@
     <t>mypluha</t>
   </si>
   <si>
-    <t>1 ч. 2 мин. 26 сек.</t>
+    <t>1 ч. 02 мин. 26 сек.</t>
   </si>
   <si>
     <t>derryne</t>
@@ -7382,7 +7382,7 @@
     <t>cross1313</t>
   </si>
   <si>
-    <t>3 ч. 28 мин. 3 сек.</t>
+    <t>3 ч. 28 мин. 03 сек.</t>
   </si>
   <si>
     <t>1018</t>
@@ -7421,7 +7421,7 @@
     <t>mtu</t>
   </si>
   <si>
-    <t>1 ч. 5 мин. 20 сек.</t>
+    <t>1 ч. 05 мин. 20 сек.</t>
   </si>
   <si>
     <t>1023</t>
@@ -7454,7 +7454,7 @@
     <t>Bimbuha</t>
   </si>
   <si>
-    <t>2 ч. 19 мин. 3 сек.</t>
+    <t>2 ч. 19 мин. 03 сек.</t>
   </si>
   <si>
     <t>Sport32brya</t>
@@ -7475,7 +7475,7 @@
     <t>безтормозов</t>
   </si>
   <si>
-    <t>5 ч. 23 мин. 8 сек.</t>
+    <t>5 ч. 23 мин. 08 сек.</t>
   </si>
   <si>
     <t>1030–1031</t>
@@ -7484,7 +7484,7 @@
     <t>mourieste</t>
   </si>
   <si>
-    <t>2 ч. 5 мин. 7 сек.</t>
+    <t>2 ч. 05 мин. 07 сек.</t>
   </si>
   <si>
     <t>Demonikus</t>
@@ -7505,7 +7505,7 @@
     <t>padfoot</t>
   </si>
   <si>
-    <t>3 ч. 23 мин. 3 сек.</t>
+    <t>3 ч. 23 мин. 03 сек.</t>
   </si>
   <si>
     <t>1034–1036</t>
@@ -7520,7 +7520,7 @@
     <t>Пилле-Рийн</t>
   </si>
   <si>
-    <t>4 ч. 27 мин. 4 сек.</t>
+    <t>4 ч. 27 мин. 04 сек.</t>
   </si>
   <si>
     <t>er1</t>
@@ -7535,7 +7535,7 @@
     <t>франс</t>
   </si>
   <si>
-    <t>1 ч. 9 мин. 3 сек.</t>
+    <t>1 ч. 09 мин. 03 сек.</t>
   </si>
   <si>
     <t>prosoeros</t>
@@ -7577,7 +7577,7 @@
     <t>RasulHacker</t>
   </si>
   <si>
-    <t>3 ч. 6 мин. 17 сек.</t>
+    <t>3 ч. 06 мин. 17 сек.</t>
   </si>
   <si>
     <t>1044</t>
@@ -7604,7 +7604,7 @@
     <t>Rsay</t>
   </si>
   <si>
-    <t>4 ч. 26 мин. 1 сек.</t>
+    <t>4 ч. 26 мин. 01 сек.</t>
   </si>
   <si>
     <t>1047–1049</t>
@@ -7658,7 +7658,7 @@
     <t>Рюша</t>
   </si>
   <si>
-    <t>9 ч. 46 мин. 1 сек.</t>
+    <t>9 ч. 46 мин. 01 сек.</t>
   </si>
   <si>
     <t>1055</t>
@@ -7712,7 +7712,7 @@
     <t>juls3n</t>
   </si>
   <si>
-    <t>13 ч. 2 мин. 20 сек.</t>
+    <t>13 ч. 02 мин. 20 сек.</t>
   </si>
   <si>
     <t>1062–1063</t>
@@ -7721,13 +7721,13 @@
     <t>AlexPolos</t>
   </si>
   <si>
-    <t>1 ч. 36 мин. 6 сек.</t>
+    <t>1 ч. 36 мин. 06 сек.</t>
   </si>
   <si>
     <t>lordoz_vladi</t>
   </si>
   <si>
-    <t>2 ч. 6 мин. 54 сек.</t>
+    <t>2 ч. 06 мин. 54 сек.</t>
   </si>
   <si>
     <t>1064</t>
@@ -7745,7 +7745,7 @@
     <t>sourses</t>
   </si>
   <si>
-    <t>6 ч. 44 мин. 6 сек.</t>
+    <t>6 ч. 44 мин. 06 сек.</t>
   </si>
   <si>
     <t>1066–1067</t>
@@ -7772,7 +7772,7 @@
     <t>trilus</t>
   </si>
   <si>
-    <t>5 ч. 55 мин. 5 сек.</t>
+    <t>5 ч. 55 мин. 05 сек.</t>
   </si>
   <si>
     <t>1070</t>
@@ -7781,7 +7781,7 @@
     <t>fpv_yo</t>
   </si>
   <si>
-    <t>1 ч. 29 мин. 5 сек.</t>
+    <t>1 ч. 29 мин. 05 сек.</t>
   </si>
   <si>
     <t>1071</t>
@@ -7805,7 +7805,7 @@
     <t>studyingtaping</t>
   </si>
   <si>
-    <t>2 ч. 5 мин. 11 сек.</t>
+    <t>2 ч. 05 мин. 11 сек.</t>
   </si>
   <si>
     <t>Boris166</t>
@@ -7919,7 +7919,7 @@
     <t>vicusto</t>
   </si>
   <si>
-    <t>2 ч. 28 мин. 0 сек.</t>
+    <t>2 ч. 28 мин. 00 сек.</t>
   </si>
   <si>
     <t>Элихи</t>
@@ -7946,13 +7946,13 @@
     <t>улиточкаЛ</t>
   </si>
   <si>
-    <t>2 ч. 9 мин. 36 сек.</t>
+    <t>2 ч. 09 мин. 36 сек.</t>
   </si>
   <si>
     <t>Lufik</t>
   </si>
   <si>
-    <t>3 ч. 29 мин. 9 сек.</t>
+    <t>3 ч. 29 мин. 09 сек.</t>
   </si>
   <si>
     <t>Dmitryi13</t>
@@ -7973,7 +7973,7 @@
     <t>Anastasilya</t>
   </si>
   <si>
-    <t>2 ч. 2 мин. 58 сек.</t>
+    <t>2 ч. 02 мин. 58 сек.</t>
   </si>
   <si>
     <t>1097–1098</t>
@@ -8006,7 +8006,7 @@
     <t>pmp</t>
   </si>
   <si>
-    <t>2 ч. 47 мин. 2 сек.</t>
+    <t>2 ч. 47 мин. 02 сек.</t>
   </si>
   <si>
     <t>1101</t>
@@ -8033,7 +8033,7 @@
     <t>dynairi</t>
   </si>
   <si>
-    <t>3 ч. 8 мин. 45 сек.</t>
+    <t>3 ч. 08 мин. 45 сек.</t>
   </si>
   <si>
     <t>1104</t>
@@ -8069,7 +8069,7 @@
     <t>St58047</t>
   </si>
   <si>
-    <t>2 ч. 44 мин. 3 сек.</t>
+    <t>2 ч. 44 мин. 03 сек.</t>
   </si>
   <si>
     <t>Mask2017</t>
@@ -8096,7 +8096,7 @@
     <t>Anna918</t>
   </si>
   <si>
-    <t>2 ч. 2 мин. 49 сек.</t>
+    <t>2 ч. 02 мин. 49 сек.</t>
   </si>
   <si>
     <t>1112</t>
@@ -8114,7 +8114,7 @@
     <t>Alexey2</t>
   </si>
   <si>
-    <t>4 ч. 30 мин. 1 сек.</t>
+    <t>4 ч. 30 мин. 01 сек.</t>
   </si>
   <si>
     <t>1114</t>
@@ -8138,7 +8138,7 @@
     <t>sh1</t>
   </si>
   <si>
-    <t>2 ч. 14 мин. 2 сек.</t>
+    <t>2 ч. 14 мин. 02 сек.</t>
   </si>
   <si>
     <t>1117</t>
@@ -8156,7 +8156,7 @@
     <t>Вася_</t>
   </si>
   <si>
-    <t>3 ч. 37 мин. 1 сек.</t>
+    <t>3 ч. 37 мин. 01 сек.</t>
   </si>
   <si>
     <t>1119</t>
@@ -8210,7 +8210,7 @@
     <t>as-83</t>
   </si>
   <si>
-    <t>2 ч. 8 мин. 51 сек.</t>
+    <t>2 ч. 08 мин. 51 сек.</t>
   </si>
   <si>
     <t>1125</t>

</xml_diff>